<commit_message>
WIP - Change Page Name to ID; change QuestionSet Name to ID; Bug when testing histology quiz; First and second page display properly - 3rd page fails.
</commit_message>
<xml_diff>
--- a/Documentation/XML LayoutAndAttributes.xlsx
+++ b/Documentation/XML LayoutAndAttributes.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BainesWork\Slicer\ImageQuizzerWork\StudyPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E760432-0BAB-4339-8758-9554CEDD9B3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="555" windowWidth="17895" windowHeight="10755" xr2:uid="{C40550C3-7968-4104-9453-4CBAFA6AC041}"/>
+    <workbookView xWindow="2160" yWindow="555" windowWidth="17895" windowHeight="10755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t>Element</t>
   </si>
@@ -44,9 +43,6 @@
     <t>Session</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Page</t>
   </si>
   <si>
@@ -101,9 +97,6 @@
     <t>Option</t>
   </si>
   <si>
-    <t>Not in demo yet</t>
-  </si>
-  <si>
     <t>(ROI name in RTStruct)</t>
   </si>
   <si>
@@ -122,9 +115,6 @@
     <t>ROIVisibilityCode</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>LinkViews</t>
   </si>
   <si>
@@ -144,9 +134,6 @@
   </si>
   <si>
     <t>Slicer defined color maps (eg. 'PET-Heat' ); these are case sensitive</t>
-  </si>
-  <si>
-    <t>UsePreviousLabelMap</t>
   </si>
   <si>
     <t>ColorTable</t>
@@ -238,9 +225,6 @@
     <t>part of previous label map name</t>
   </si>
   <si>
-    <t>searches for latest labelmap file that matches Page Name+Descriptor+ '-bainesquizlabel.nrrd'</t>
-  </si>
-  <si>
     <t>DicomFormat</t>
   </si>
   <si>
@@ -263,12 +247,39 @@
   </si>
   <si>
     <t>moved to post processing as input variable - to remap RTSTruct to original dicom UID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… </t>
+  </si>
+  <si>
+    <t>DisplayLabelMapID</t>
+  </si>
+  <si>
+    <t>LabelMapID</t>
+  </si>
+  <si>
+    <t>searches history for an image with a LabelMapID attribute that matches this string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only used in the progress bar label - mostly used when editing the xml for convenience </t>
+  </si>
+  <si>
+    <t>ID string used for matching if subsequent Image needs this Label Map displayed</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>LabelMapPath</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -402,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -428,7 +439,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,11 +756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD49616-A605-4867-9792-E0F0E8F07DBB}">
-  <dimension ref="A1:J34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,64 +770,60 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="99" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="73.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="40" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="8">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44491</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44515</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -822,498 +832,487 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="13"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+      <c r="H20" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
+      <c r="H21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
+      <c r="H22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="14" t="s">
-        <v>56</v>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="15" t="s">
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J23" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>10</v>
+      <c r="D24" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="13"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="13"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="2"/>
+      <c r="H26" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="13"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="13"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J32" s="13"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J33" s="13"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="13"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
XML updates for ID and LabelMapID logic
</commit_message>
<xml_diff>
--- a/Documentation/XML LayoutAndAttributes.xlsx
+++ b/Documentation/XML LayoutAndAttributes.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t>Element</t>
   </si>
@@ -225,15 +225,9 @@
     <t>part of previous label map name</t>
   </si>
   <si>
-    <t>DicomFormat</t>
-  </si>
-  <si>
     <t>if DicomFormat=Y, path to one slice of the DICOM series</t>
   </si>
   <si>
-    <t>all other formats read in as a 'Data' volume (NRRD, NIFTI, MHD)</t>
-  </si>
-  <si>
     <t>eg. Pi-RadsStudy.txt, LungSABRStudy.txt, GenericColors.txt (default)</t>
   </si>
   <si>
@@ -274,6 +268,15 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>DicomRead</t>
+  </si>
+  <si>
+    <t>all other formats read in as a 'Data' volume (NRRD, NIFTI, MHD) ; Even a dicom slice can be read in as a Data volume by setting this to 'N' and setting the attribute 'Type' to 'Volume'</t>
+  </si>
+  <si>
+    <t>text to appear as option in the question</t>
   </si>
 </sst>
 </file>
@@ -759,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +788,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44515</v>
+        <v>44516</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -836,10 +839,10 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -871,7 +874,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -904,10 +907,10 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -944,14 +947,14 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>39</v>
@@ -960,7 +963,7 @@
         <v>36</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -987,14 +990,14 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1004,14 +1007,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1055,7 +1058,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="2"/>
       <c r="H20" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I20" s="13"/>
     </row>
@@ -1103,7 +1106,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1120,7 +1123,7 @@
         <v>53</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1293,25 +1296,29 @@
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>4</v>
       </c>
-      <c r="F41" t="s">
-        <v>70</v>
+      <c r="D41" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F42" t="s">
-        <v>71</v>
+      <c r="D42" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on validation code for XML elements and attributes.
</commit_message>
<xml_diff>
--- a/Documentation/XML LayoutAndAttributes.xlsx
+++ b/Documentation/XML LayoutAndAttributes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BainesWork\Slicer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A852F17-64EC-47EC-B174-A863626F6482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="555" windowWidth="17895" windowHeight="10755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>Element</t>
   </si>
@@ -100,12 +102,6 @@
     <t>(ROI name in RTStruct)</t>
   </si>
   <si>
-    <t>Axial, Sagittal, Coronal</t>
-  </si>
-  <si>
-    <t>Foreground, Background, Label</t>
-  </si>
-  <si>
     <t>(relative path to image data file)</t>
   </si>
   <si>
@@ -131,9 +127,6 @@
   </si>
   <si>
     <t>AllowMultipleResponses</t>
-  </si>
-  <si>
-    <t>Slicer defined color maps (eg. 'PET-Heat' ); these are case sensitive</t>
   </si>
   <si>
     <t>ColorTable</t>
@@ -237,9 +230,6 @@
     <t>Not yet complete</t>
   </si>
   <si>
-    <t>Red, Green, Yellow, Slice4</t>
-  </si>
-  <si>
     <t>moved to post processing as input variable - to remap RTSTruct to original dicom UID</t>
   </si>
   <si>
@@ -273,16 +263,37 @@
     <t>DicomRead</t>
   </si>
   <si>
-    <t>all other formats read in as a 'Data' volume (NRRD, NIFTI, MHD) ; Even a dicom slice can be read in as a Data volume by setting this to 'N' and setting the attribute 'Type' to 'Volume'</t>
-  </si>
-  <si>
     <t>text to appear as option in the question</t>
+  </si>
+  <si>
+    <t>Foreground, Background, Label (default=Background)</t>
+  </si>
+  <si>
+    <t>Axial, Sagittal, Coronal (default=Axial)</t>
+  </si>
+  <si>
+    <t>Red, Green, Yellow, Slice4 (default=Red)</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>TwoOverTwo, FourUp, OneUpRedSlice, SideBySideRedYellow (default=TwoOverTwo)</t>
+  </si>
+  <si>
+    <t>all other formats read in as a 'Data' volume (NRRD, NIFTI, MHD...) ; Even a dicom slice can be read in as a Data volume by setting this to 'N' and setting the attribute 'Type' to 'Volume'</t>
+  </si>
+  <si>
+    <t>view Slicer MRML nodes to get Slicer's list; these are case sensitive</t>
+  </si>
+  <si>
+    <t>Slicer defined color maps (eg. 'PET-Heat' ) default=Grey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -446,6 +457,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,11 +771,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,26 +786,26 @@
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
     <col min="8" max="8" width="73.85546875" style="11" customWidth="1"/>
     <col min="9" max="9" width="40" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44516</v>
+        <v>44522</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -817,13 +829,13 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -835,14 +847,14 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -852,11 +864,11 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I8" s="12"/>
     </row>
@@ -867,14 +879,14 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -886,14 +898,14 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -903,14 +915,14 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -920,117 +932,117 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>39</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="13" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="16"/>
+        <v>27</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="H16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="G17" s="16"/>
       <c r="H17" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="13"/>
+        <v>16</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1039,7 +1051,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="13" t="s">
@@ -1047,33 +1059,35 @@
       </c>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="13"/>
+        <v>76</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="1"/>
       <c r="G21" s="2"/>
       <c r="H21" s="13" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="I21" s="13"/>
     </row>
@@ -1082,109 +1096,111 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
       <c r="H22" s="13" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
       <c r="H23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>56</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="14" t="s">
-        <v>52</v>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="15" t="s">
+      <c r="G24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I24" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>9</v>
+      <c r="D25" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I25" s="13"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="H26" s="13" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="E27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="13" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="13" t="s">
@@ -1199,11 +1215,11 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="13" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="I29" s="13"/>
     </row>
@@ -1214,11 +1230,11 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I30" s="13"/>
     </row>
@@ -1226,16 +1242,14 @@
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="13" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="I31" s="13"/>
     </row>
@@ -1243,16 +1257,16 @@
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G32" s="2"/>
       <c r="H32" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I32" s="13"/>
     </row>
@@ -1263,11 +1277,13 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="H33" s="13" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="I33" s="13"/>
     </row>
@@ -1278,11 +1294,11 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I34" s="13"/>
     </row>
@@ -1291,34 +1307,49 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="1"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="I36" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>4</v>
       </c>
-      <c r="D41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update validation code; fix coding convention for 'GetChildren' - this returns a list of xml elements - prefixed my variables with an 'l'; (TODO - GetChildren in Session code); Added more examples for TestHistology quiz
</commit_message>
<xml_diff>
--- a/Documentation/XML LayoutAndAttributes.xlsx
+++ b/Documentation/XML LayoutAndAttributes.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BainesWork\Slicer\ImageQuizzerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A852F17-64EC-47EC-B174-A863626F6482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
   <si>
     <t>Element</t>
   </si>
@@ -171,8 +170,92 @@
     <t>ID</t>
   </si>
   <si>
+    <t>… (numbers not recommended in case you have to randomize the pages)</t>
+  </si>
+  <si>
+    <t>OriginalDicomDir</t>
+  </si>
+  <si>
+    <t>(relative path to original folder holding dicom series)</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>if DicomFormat=Y, path to one slice of the DICOM series</t>
+  </si>
+  <si>
+    <t>eg. Pi-RadsStudy.txt, LungSABRStudy.txt, GenericColors.txt (default)</t>
+  </si>
+  <si>
+    <t>syntax: number descriptor r g b a</t>
+  </si>
+  <si>
+    <t>moved to post processing as input variable - to remap RTSTruct to original dicom UID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… </t>
+  </si>
+  <si>
+    <t>DisplayLabelMapID</t>
+  </si>
+  <si>
+    <t>LabelMapID</t>
+  </si>
+  <si>
+    <t>searches history for an image with a LabelMapID attribute that matches this string</t>
+  </si>
+  <si>
+    <t>ID string used for matching if subsequent Image needs this Label Map displayed</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>LabelMapPath</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>DicomRead</t>
+  </si>
+  <si>
+    <t>text to appear as option in the question</t>
+  </si>
+  <si>
+    <t>Foreground, Background, Label (default=Background)</t>
+  </si>
+  <si>
+    <t>Axial, Sagittal, Coronal (default=Axial)</t>
+  </si>
+  <si>
+    <t>Red, Green, Yellow, Slice4 (default=Red)</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>TwoOverTwo, FourUp, OneUpRedSlice, SideBySideRedYellow (default=TwoOverTwo)</t>
+  </si>
+  <si>
+    <t>all other formats read in as a 'Data' volume (NRRD, NIFTI, MHD...) ; Even a dicom slice can be read in as a Data volume by setting this to 'N' and setting the attribute 'Type' to 'Volume'</t>
+  </si>
+  <si>
+    <t>view Slicer MRML nodes to get Slicer's list; these are case sensitive</t>
+  </si>
+  <si>
+    <t>Slicer defined color maps (eg. 'PET-Heat' ) default=Grey</t>
+  </si>
+  <si>
+    <t>this combines with Image ID to create a unique node name when loaded into Slicer</t>
+  </si>
+  <si>
+    <t>this combines with Page ID to create a unique  node name when loaded into Slicer</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">(different for each </t>
+      <t xml:space="preserve">… (different for each </t>
     </r>
     <r>
       <rPr>
@@ -197,103 +280,16 @@
     </r>
   </si>
   <si>
-    <t>… (numbers not recommended in case you have to randomize the pages)</t>
-  </si>
-  <si>
-    <t>SaveLabelMapAsRTStruct</t>
-  </si>
-  <si>
-    <t>MapRTStructToVolume</t>
-  </si>
-  <si>
-    <t>OriginalDicomDir</t>
-  </si>
-  <si>
-    <t>(relative path to original folder holding dicom series)</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>part of previous label map name</t>
-  </si>
-  <si>
-    <t>if DicomFormat=Y, path to one slice of the DICOM series</t>
-  </si>
-  <si>
-    <t>eg. Pi-RadsStudy.txt, LungSABRStudy.txt, GenericColors.txt (default)</t>
-  </si>
-  <si>
-    <t>syntax: number descriptor r g b a</t>
-  </si>
-  <si>
-    <t>Not yet complete</t>
-  </si>
-  <si>
-    <t>moved to post processing as input variable - to remap RTSTruct to original dicom UID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… </t>
-  </si>
-  <si>
-    <t>DisplayLabelMapID</t>
-  </si>
-  <si>
-    <t>LabelMapID</t>
-  </si>
-  <si>
-    <t>searches history for an image with a LabelMapID attribute that matches this string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">only used in the progress bar label - mostly used when editing the xml for convenience </t>
-  </si>
-  <si>
-    <t>ID string used for matching if subsequent Image needs this Label Map displayed</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>LabelMapPath</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>DicomRead</t>
-  </si>
-  <si>
-    <t>text to appear as option in the question</t>
-  </si>
-  <si>
-    <t>Foreground, Background, Label (default=Background)</t>
-  </si>
-  <si>
-    <t>Axial, Sagittal, Coronal (default=Axial)</t>
-  </si>
-  <si>
-    <t>Red, Green, Yellow, Slice4 (default=Red)</t>
-  </si>
-  <si>
-    <t>Layout</t>
-  </si>
-  <si>
-    <t>TwoOverTwo, FourUp, OneUpRedSlice, SideBySideRedYellow (default=TwoOverTwo)</t>
-  </si>
-  <si>
-    <t>all other formats read in as a 'Data' volume (NRRD, NIFTI, MHD...) ; Even a dicom slice can be read in as a Data volume by setting this to 'N' and setting the attribute 'Type' to 'Volume'</t>
-  </si>
-  <si>
-    <t>view Slicer MRML nodes to get Slicer's list; these are case sensitive</t>
-  </si>
-  <si>
-    <t>Slicer defined color maps (eg. 'PET-Heat' ) default=Grey</t>
+    <t>only used in the progress bar label - mostly used for convenience when editing the xml</t>
+  </si>
+  <si>
+    <t>required for RTStruct type of image</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,12 +358,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -439,7 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -771,11 +760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,8 +776,8 @@
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.85546875" customWidth="1"/>
-    <col min="8" max="8" width="73.85546875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="40" style="11" customWidth="1"/>
+    <col min="8" max="8" width="73.85546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="40" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -800,7 +789,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44522</v>
+        <v>44523</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -834,8 +823,8 @@
       <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>51</v>
+      <c r="I6" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -850,11 +839,11 @@
         <v>43</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>55</v>
+      <c r="H7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -863,14 +852,10 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="12"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -878,18 +863,12 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -900,12 +879,14 @@
       <c r="F10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>52</v>
+      <c r="G10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -918,11 +899,11 @@
         <v>26</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>62</v>
+      <c r="H11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -935,10 +916,10 @@
         <v>25</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -947,15 +928,15 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -966,13 +947,15 @@
       <c r="F14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="13"/>
+      <c r="H14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -981,16 +964,14 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>74</v>
+      <c r="I15" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1005,10 +986,10 @@
       <c r="G16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="13"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1017,14 +998,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="13" t="s">
-        <v>63</v>
+      <c r="I17" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1034,14 +1015,14 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="13" t="s">
-        <v>61</v>
+      <c r="I18" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1054,10 +1035,10 @@
         <v>28</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="13"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -1069,11 +1050,11 @@
         <v>31</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>75</v>
+      <c r="H20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1086,10 +1067,10 @@
       <c r="E21" s="2"/>
       <c r="F21" s="1"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" s="13"/>
+      <c r="H21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -1101,10 +1082,10 @@
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I22" s="13"/>
+      <c r="H22" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1116,10 +1097,10 @@
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" s="13"/>
+      <c r="H23" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1130,31 +1111,31 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="13" t="s">
-        <v>53</v>
+      <c r="I24" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="14" t="s">
-        <v>49</v>
+      <c r="D25" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>57</v>
+      <c r="H25" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1171,10 +1152,12 @@
       <c r="G26" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I26" s="13"/>
+      <c r="I26" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -1186,10 +1169,10 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="13"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1203,10 +1186,10 @@
         <v>44</v>
       </c>
       <c r="G28" s="2"/>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="13"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -1218,10 +1201,10 @@
         <v>26</v>
       </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="13"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1233,10 +1216,10 @@
         <v>29</v>
       </c>
       <c r="G30" s="2"/>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="13"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -1248,10 +1231,10 @@
         <v>30</v>
       </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I31" s="13"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1265,10 +1248,10 @@
         <v>26</v>
       </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="13"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -1282,10 +1265,10 @@
       <c r="G33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="13"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -1297,10 +1280,10 @@
         <v>37</v>
       </c>
       <c r="G34" s="2"/>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="13"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -1312,10 +1295,10 @@
         <v>38</v>
       </c>
       <c r="G35" s="2"/>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I35" s="13"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -1327,11 +1310,11 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="13" t="s">
-        <v>68</v>
+      <c r="I36" s="12" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1339,17 +1322,17 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added LogoutTime code; Added shareable Slicer volume Panoramix-cropped - for Pancreas type of image data
</commit_message>
<xml_diff>
--- a/Documentation/XML LayoutAndAttributes.xlsx
+++ b/Documentation/XML LayoutAndAttributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71573D02-954A-4CC9-998D-8653E2E1CE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5373691A-4E5D-4770-9C8C-4DAE060AEB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3312" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
   <si>
     <t>Element</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>SegmentRequired</t>
-  </si>
-  <si>
-    <t>AllowMultipleResponses</t>
   </si>
   <si>
     <t>ColorTable</t>
@@ -363,6 +360,15 @@
   </si>
   <si>
     <t>SubElement2</t>
+  </si>
+  <si>
+    <t>AllowMultipleResponse</t>
+  </si>
+  <si>
+    <t>LogoutTime</t>
+  </si>
+  <si>
+    <t>logout timestamp reflecting the last time a save was done to the user's response xml</t>
   </si>
 </sst>
 </file>
@@ -835,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,19 +862,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44588</v>
+        <v>44589</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -892,13 +898,13 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -910,14 +916,14 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
@@ -927,14 +933,14 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -946,16 +952,16 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>44</v>
-      </c>
       <c r="I9" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -969,10 +975,10 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -986,10 +992,10 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -999,11 +1005,11 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I12" s="12"/>
     </row>
@@ -1014,14 +1020,14 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1033,16 +1039,16 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1052,14 +1058,14 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1072,7 +1078,7 @@
         <v>26</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>17</v>
@@ -1086,14 +1092,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1103,14 +1109,14 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1124,7 +1130,7 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" s="12"/>
     </row>
@@ -1135,14 +1141,14 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1156,7 +1162,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="2"/>
       <c r="H21" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I21" s="12"/>
     </row>
@@ -1171,7 +1177,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I22" s="12"/>
     </row>
@@ -1186,7 +1192,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
       <c r="H23" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I23" s="12"/>
     </row>
@@ -1200,13 +1206,13 @@
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
       <c r="G24" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1221,13 +1227,13 @@
         <v>23</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1244,7 +1250,7 @@
         <v>21</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1256,14 +1262,14 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1280,7 +1286,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1294,10 +1300,10 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -1307,14 +1313,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="1" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1333,7 +1339,7 @@
         <v>16</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1346,7 +1352,7 @@
         <v>26</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>19</v>
@@ -1360,11 +1366,11 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I33" s="12"/>
     </row>
@@ -1375,11 +1381,11 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I34" s="12"/>
     </row>
@@ -1397,7 +1403,7 @@
         <v>16</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1424,33 +1430,33 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -1458,10 +1464,10 @@
         <v>0</v>
       </c>
       <c r="D42" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>97</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>1</v>
@@ -1474,26 +1480,26 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -1504,23 +1510,23 @@
         <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.3">
@@ -1528,18 +1534,29 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
+        <v>71</v>
+      </c>
+      <c r="H52" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="F53" t="s">
+        <v>69</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>